<commit_message>
for updated version of the paper
</commit_message>
<xml_diff>
--- a/Paper data algorithm.xlsx
+++ b/Paper data algorithm.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/718232a78c2c86d3/Documenten/uni/uni documenten/MEP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2261" documentId="8_{E17B2787-9971-40C2-91F6-032D716F4A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF8C14D0-5335-4E09-B613-63004E449F71}"/>
+  <xr:revisionPtr revIDLastSave="2562" documentId="8_{E17B2787-9971-40C2-91F6-032D716F4A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C481B14A-FFF4-44C6-9A07-228C88423BA9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{76006F6F-BB6B-4FCD-8E2D-5E202D6EDD84}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{76006F6F-BB6B-4FCD-8E2D-5E202D6EDD84}"/>
   </bookViews>
   <sheets>
     <sheet name="noise" sheetId="1" r:id="rId1"/>
     <sheet name="resolution" sheetId="2" r:id="rId2"/>
-    <sheet name="temps+inits" sheetId="3" r:id="rId3"/>
-    <sheet name="num metrics" sheetId="4" r:id="rId4"/>
-    <sheet name="optimization" sheetId="6" r:id="rId5"/>
-    <sheet name="right&amp;wrong" sheetId="5" r:id="rId6"/>
+    <sheet name="optimization revised" sheetId="7" r:id="rId3"/>
+    <sheet name="temps+inits" sheetId="3" r:id="rId4"/>
+    <sheet name="num metrics" sheetId="4" r:id="rId5"/>
+    <sheet name="optimization" sheetId="6" r:id="rId6"/>
+    <sheet name="right&amp;wrong" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="158">
   <si>
     <t>stat/var noise</t>
   </si>
@@ -424,15 +425,154 @@
   <si>
     <t>Score for true system</t>
   </si>
+  <si>
+    <t>Double iterations</t>
+  </si>
+  <si>
+    <t>triple iterations</t>
+  </si>
+  <si>
+    <t>Double iter</t>
+  </si>
+  <si>
+    <t>Triple iter</t>
+  </si>
+  <si>
+    <t>#SMAPE 0.1 results</t>
+  </si>
+  <si>
+    <t>#SMAPE 0.2 results</t>
+  </si>
+  <si>
+    <t>#SMAPE 0.4 results</t>
+  </si>
+  <si>
+    <t>Chemfit parameters for a SMAPE of 0.05</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>16716</t>
+  </si>
+  <si>
+    <t>14893</t>
+  </si>
+  <si>
+    <t>18431</t>
+  </si>
+  <si>
+    <t>15589</t>
+  </si>
+  <si>
+    <t>12232</t>
+  </si>
+  <si>
+    <t>24725</t>
+  </si>
+  <si>
+    <t>21096</t>
+  </si>
+  <si>
+    <t>11225</t>
+  </si>
+  <si>
+    <t>12755</t>
+  </si>
+  <si>
+    <t>13550</t>
+  </si>
+  <si>
+    <t>24555</t>
+  </si>
+  <si>
+    <t>14247</t>
+  </si>
+  <si>
+    <t>19395</t>
+  </si>
+  <si>
+    <t>22674</t>
+  </si>
+  <si>
+    <t>28023</t>
+  </si>
+  <si>
+    <t>12455</t>
+  </si>
+  <si>
+    <t>35554</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>yield</t>
+  </si>
+  <si>
+    <t>cat conc</t>
+  </si>
+  <si>
+    <t>pressure</t>
+  </si>
+  <si>
+    <t>substrate conc</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>True parameters</t>
+  </si>
+  <si>
+    <t>SMAPE 0,05</t>
+  </si>
+  <si>
+    <t>SMAPE 0,10</t>
+  </si>
+  <si>
+    <t>SMAPE 0,20</t>
+  </si>
+  <si>
+    <t>SMAPE 0,4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.00000000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -749,7 +889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -844,9 +984,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -876,7 +1018,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -938,7 +1080,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -988,10 +1130,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>resolution!$K$2:$K$13</c:f>
+              <c:f>resolution!$K$2:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>120</c:v>
                 </c:pt>
@@ -1024,19 +1166,16 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>resolution!$L$2:$L$13</c:f>
+              <c:f>resolution!$L$2:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>9.9069306164461402E-3</c:v>
                 </c:pt>
@@ -1069,9 +1208,6 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>7.4038794524886195E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.30262494241506599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1123,10 +1259,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>resolution!$K$2:$K$13</c:f>
+              <c:f>resolution!$K$2:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>120</c:v>
                 </c:pt>
@@ -1159,19 +1295,16 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>resolution!$M$2:$M$13</c:f>
+              <c:f>resolution!$M$2:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.15184317161043559</c:v>
                 </c:pt>
@@ -1204,9 +1337,6 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.2901396885429634</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.28560059863407572</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1215,6 +1345,219 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8BCE-4FCF-9F3E-37A65F1984D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resolution!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Double iter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>resolution!$K$2:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>resolution!$N$2:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.5892299346689135E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5602152249516387E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6273886462089043E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10146021097734037</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13722927374678071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AB29-4665-A1B1-BF16A0937D54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resolution!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Triple iter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>resolution!$K$2:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>resolution!$O$2:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.4840100173685939E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2173074449784987E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AB29-4665-A1B1-BF16A0937D54}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1302,7 +1645,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1340,7 +1683,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718606680"/>
@@ -1419,7 +1762,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1457,7 +1800,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718606352"/>
@@ -1499,7 +1842,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1536,7 +1879,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1550,7 +1893,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1617,7 +1960,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1661,19 +2004,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>0.12826232002703686</c:v>
+                  <c:v>0.47660734054882703</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11521577061171033</c:v>
+                  <c:v>0.11011067595292796</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10111266851354897</c:v>
+                  <c:v>0.13554706334072611</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14652123282950061</c:v>
+                  <c:v>0.12262126794396215</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16997368084976899</c:v>
+                  <c:v>0.12480658983983366</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,7 +2190,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1884,7 +2227,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718065736"/>
@@ -1964,7 +2307,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2002,7 +2345,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718068360"/>
@@ -2050,7 +2393,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2064,7 +2407,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2159,7 +2502,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2203,22 +2546,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="1">
-                  <c:v>0.32441322556399999</c:v>
+                  <c:v>0.38968565539956995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14288735612172593</c:v>
+                  <c:v>0.15337633108682519</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.585879661580508E-2</c:v>
+                  <c:v>0.12475587776439716</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27532299373945446</c:v>
+                  <c:v>7.212470049680561E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.41375338285357915</c:v>
+                  <c:v>5.9463932486319392E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5637408299033464</c:v>
+                  <c:v>4.6079164035784957E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2390,7 +2733,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2427,7 +2770,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="653071328"/>
@@ -2506,7 +2849,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2544,7 +2887,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="653071000"/>
@@ -2592,7 +2935,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2606,7 +2949,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2643,7 +2986,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3328,7 +3671,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="688023240"/>
@@ -3387,7 +3730,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="688026520"/>
@@ -3429,7 +3772,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3466,7 +3809,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5913,8 +6256,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7063,18 +7410,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B1E574-918A-43D0-93C9-C767A11D8FF9}">
-  <dimension ref="A1:Z29"/>
+  <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:Z3"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R5" sqref="Q5:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="12" max="12" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -7087,8 +7435,14 @@
       <c r="M1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="N1" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>120</v>
       </c>
@@ -7118,45 +7472,53 @@
         <f>AVERAGE(B15:F15)</f>
         <v>0.15184317161043559</v>
       </c>
-      <c r="O2" cm="1">
-        <f t="array" ref="O2:Z3">TRANSPOSE(L2:M13)</f>
+      <c r="N2">
+        <f>AVERAGE(B29:F29)</f>
+        <v>5.5892299346689135E-2</v>
+      </c>
+      <c r="O2">
+        <f>AVERAGE(B36:F36)</f>
+        <v>3.4840100173685939E-2</v>
+      </c>
+      <c r="Q2" cm="1">
+        <f t="array" ref="Q2:AB5">TRANSPOSE(L2:O13)</f>
         <v>9.9069306164461402E-3</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>1.9077525198916999E-2</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>2.1075758971819299E-2</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>3.5933315828482124E-2</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>2.5965459400004564E-2</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>3.7405057350412038E-2</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>5.3036896068016003E-2</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>4.5773000409559797E-2</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>5.2234662828366897E-2</v>
       </c>
-      <c r="X2">
+      <c r="Z2">
         <v>0.120728141436048</v>
       </c>
-      <c r="Y2">
+      <c r="AA2">
         <v>7.4038794524886195E-2</v>
       </c>
-      <c r="Z2">
+      <c r="AB2">
         <v>0.30262494241506599</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>60</v>
       </c>
@@ -7186,44 +7548,52 @@
         <f t="shared" ref="M3:M13" si="1">AVERAGE(B16:F16)</f>
         <v>0.102350495769891</v>
       </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N4" si="2">AVERAGE(B30:F30)</f>
+        <v>4.5602152249516387E-2</v>
+      </c>
       <c r="O3">
+        <f>AVERAGE(B37:F37)</f>
+        <v>5.2173074449784987E-2</v>
+      </c>
+      <c r="Q3">
         <v>0.15184317161043559</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>0.102350495769891</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>9.0212364833213848E-2</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>0.10222289006575935</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>0.13154454769095564</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>0.1380056493489962</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <v>0.12829677436831735</v>
       </c>
-      <c r="V3">
+      <c r="X3">
         <v>0.13536845499994438</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <v>0.2826345705229984</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <v>0.23483273174420888</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>0.2901396885429634</v>
       </c>
-      <c r="Z3">
+      <c r="AB3">
         <v>0.28560059863407572</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
@@ -7253,8 +7623,48 @@
         <f t="shared" si="1"/>
         <v>9.0212364833213848E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>5.6273886462089043E-2</v>
+      </c>
+      <c r="Q4">
+        <v>5.5892299346689135E-2</v>
+      </c>
+      <c r="R4">
+        <v>4.5602152249516387E-2</v>
+      </c>
+      <c r="S4">
+        <v>5.6273886462089043E-2</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0.10146021097734037</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0.13722927374678071</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>25</v>
       </c>
@@ -7284,8 +7694,44 @@
         <f t="shared" si="1"/>
         <v>0.10222289006575935</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Q5">
+        <v>3.4840100173685939E-2</v>
+      </c>
+      <c r="R5">
+        <v>5.2173074449784987E-2</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20</v>
       </c>
@@ -7316,7 +7762,7 @@
         <v>0.13154454769095564</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>15</v>
       </c>
@@ -7346,8 +7792,12 @@
         <f t="shared" si="1"/>
         <v>0.1380056493489962</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="N7">
+        <f>AVERAGE(B32:F32)</f>
+        <v>0.10146021097734037</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
@@ -7378,7 +7828,7 @@
         <v>0.12829677436831735</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7408,8 +7858,12 @@
         <f t="shared" si="1"/>
         <v>0.13536845499994438</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <f>AVERAGE(B33:F33)</f>
+        <v>0.13722927374678071</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -7440,7 +7894,7 @@
         <v>0.2826345705229984</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -7471,7 +7925,7 @@
         <v>0.23483273174420888</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
@@ -7502,7 +7956,7 @@
         <v>0.2901396885429634</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -7533,12 +7987,12 @@
         <v>0.28560059863407572</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>120</v>
       </c>
@@ -7558,7 +8012,7 @@
         <v>0.18089594150018901</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>60</v>
       </c>
@@ -7778,12 +8232,155 @@
         <v>8.8135208074904603E-2</v>
       </c>
     </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="A29">
+        <v>120</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6.0776284874391198E-2</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4.0230590071408799E-2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>8.0670378581654795E-2</v>
+      </c>
+      <c r="E29" s="1">
+        <v>6.9328505660221806E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2.8455737545769098E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1">
+        <v>4.5692758027233001E-2</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3.6356991775736799E-2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>6.2280883904184903E-2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3.1061277676646501E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>5.2618849863780702E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>5.4644962601521803E-2</v>
+      </c>
+      <c r="C31" s="1">
+        <v>7.8354039849733298E-2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3.3063891388189499E-2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4.4105702800082199E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <v>7.1200835670918394E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32" s="1">
+        <v>5.7104750677369899E-2</v>
+      </c>
+      <c r="C32" s="1">
+        <v>6.7770013850707703E-2</v>
+      </c>
+      <c r="D32" s="1">
+        <v>4.0686977880168299E-2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.184739173615421</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.15700013886303499</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.13883319097482799</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.15868218691062699</v>
+      </c>
+      <c r="D33" s="1">
+        <v>9.9446665779917606E-2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.118764957611982</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.17041936745654901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>120</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2.4728097479248499E-2</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2.93592467550042E-2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1.8120420990648201E-2</v>
+      </c>
+      <c r="E36" s="1">
+        <v>6.1660616586454199E-2</v>
+      </c>
+      <c r="F36" s="1">
+        <v>4.0332119057074602E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>60</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2.9922403858221799E-2</v>
+      </c>
+      <c r="C37" s="1">
+        <v>5.42980200042096E-2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>5.5705359528884002E-2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3.09711762972831E-2</v>
+      </c>
+      <c r="F37" s="1">
+        <v>8.9968412560326394E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7793,11 +8390,431 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB486C5-C788-456E-AE38-E770553E351F}">
+  <dimension ref="A1:K55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="39">
+        <v>3.335</v>
+      </c>
+      <c r="G2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H2" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="39">
+        <v>1.98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="H3">
+        <v>0.48080000000000001</v>
+      </c>
+      <c r="I3">
+        <v>50</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>396.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="39">
+        <v>1.2589999999999999</v>
+      </c>
+      <c r="F4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4">
+        <v>0.79090000000000005</v>
+      </c>
+      <c r="H4">
+        <v>0.50649999999999995</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>406.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="39">
+        <v>4.0990000000000002</v>
+      </c>
+      <c r="F5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="H5">
+        <v>0.57969999999999999</v>
+      </c>
+      <c r="I5">
+        <v>50</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>387.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="39">
+        <v>1.921</v>
+      </c>
+      <c r="F6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6">
+        <v>0.93759999999999999</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <v>50</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="38">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="F7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7">
+        <v>0.81679999999999997</v>
+      </c>
+      <c r="H7">
+        <v>0.16350000000000001</v>
+      </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>327.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8">
+        <v>17041</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9">
+        <v>14699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10">
+        <v>17180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11">
+        <v>11794</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12">
+        <v>12290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13">
+        <v>23902</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>3.036</v>
+      </c>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2.1520000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1.946</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18.32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1.8879999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>48.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>13.92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0.56899999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2.8959999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>40.78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>5806</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1.3740000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>8.0719999999999992</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>5.7439999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1.966</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BECF976-1F9D-4521-BFCB-8389D9F3AE5F}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7815,19 +8832,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>0.15794782190330101</v>
+        <v>0.45001318515774102</v>
       </c>
       <c r="C2" s="1">
-        <v>0.135929624025662</v>
+        <v>0.451111005796686</v>
       </c>
       <c r="D2" s="1">
-        <v>0.124953451942575</v>
+        <v>0.51519663046880404</v>
       </c>
       <c r="E2" s="1">
-        <v>0.12896263949139999</v>
+        <v>0.54589874080093403</v>
       </c>
       <c r="F2" s="1">
-        <v>9.3518062772246294E-2</v>
+        <v>0.42081714051996999</v>
       </c>
       <c r="I2">
         <v>363.39299999999997</v>
@@ -7837,20 +8854,20 @@
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>0.15135796075552699</v>
+      <c r="B3" s="1">
+        <v>4.2905398699690699E-2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.105007070406527</v>
+        <v>0.119204489253286</v>
       </c>
       <c r="D3" s="1">
-        <v>9.5401381060959897E-2</v>
+        <v>0.161434982649105</v>
       </c>
       <c r="E3" s="1">
-        <v>5.7004650254663801E-2</v>
+        <v>9.6502101484839106E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>0.167307790580874</v>
+        <v>0.13050640767771901</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
@@ -7860,20 +8877,20 @@
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>0.10354473058275999</v>
+      <c r="B4" s="1">
+        <v>6.0849093685008099E-2</v>
       </c>
       <c r="C4" s="1">
-        <v>0.13345832691191101</v>
+        <v>0.156610526030558</v>
       </c>
       <c r="D4" s="1">
-        <v>5.7627767914828397E-2</v>
+        <v>0.174373660446316</v>
       </c>
       <c r="E4" s="1">
-        <v>5.44234707844145E-2</v>
+        <v>9.3212351034178395E-2</v>
       </c>
       <c r="F4" s="1">
-        <v>0.15650904637383101</v>
+        <v>0.19268968550757001</v>
       </c>
       <c r="I4" t="s">
         <v>20</v>
@@ -7883,20 +8900,20 @@
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>0.19029847657617399</v>
+      <c r="B5" s="1">
+        <v>0.17639374508299499</v>
       </c>
       <c r="C5" s="1">
-        <v>0.132628257675839</v>
+        <v>8.9200853387824505E-2</v>
       </c>
       <c r="D5" s="1">
-        <v>0.143963903523943</v>
+        <v>0.14301509580456301</v>
       </c>
       <c r="E5" s="1">
-        <v>0.14145528030861501</v>
+        <v>0.11020204974744099</v>
       </c>
       <c r="F5" s="1">
-        <v>0.124260246062932</v>
+        <v>9.4294595696987296E-2</v>
       </c>
       <c r="I5" t="s">
         <v>21</v>
@@ -7906,20 +8923,20 @@
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>0.176954265049521</v>
+      <c r="B6" s="1">
+        <v>0.102792690730237</v>
       </c>
       <c r="C6" s="1">
-        <v>0.275619628560764</v>
+        <v>0.104030767381089</v>
       </c>
       <c r="D6" s="1">
-        <v>0.123852896654535</v>
+        <v>0.18112636036377999</v>
       </c>
       <c r="E6" s="1">
-        <v>0.16236967387731499</v>
+        <v>0.16226486287007699</v>
       </c>
       <c r="F6" s="1">
-        <v>0.11107194010671</v>
+        <v>7.3818267853985306E-2</v>
       </c>
       <c r="I6" t="s">
         <v>22</v>
@@ -7934,20 +8951,20 @@
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9">
-        <v>0.28130613318018299</v>
+      <c r="B9" s="1">
+        <v>0.305099204962472</v>
       </c>
       <c r="C9" s="1">
-        <v>0.27609094167620701</v>
+        <v>0.44407054607834401</v>
       </c>
       <c r="D9" s="1">
-        <v>0.34363120854850399</v>
+        <v>0.40911367953584599</v>
       </c>
       <c r="E9" s="1">
-        <v>0.32686950657540498</v>
+        <v>0.377778342613378</v>
       </c>
       <c r="F9" s="1">
-        <v>0.39416833783970101</v>
+        <v>0.41236650380780998</v>
       </c>
       <c r="I9" t="s">
         <v>31</v>
@@ -7957,100 +8974,100 @@
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10">
-        <v>0.14761230951581999</v>
+      <c r="B10" s="1">
+        <v>0.113788948412263</v>
       </c>
       <c r="C10" s="1">
-        <v>0.223577999164978</v>
+        <v>8.3113454945618906E-2</v>
       </c>
       <c r="D10" s="1">
-        <v>0.11786896607290701</v>
+        <v>0.12551949139320501</v>
       </c>
       <c r="E10" s="1">
-        <v>6.4223621305173603E-2</v>
+        <v>0.19960819266004301</v>
       </c>
       <c r="F10" s="1">
-        <v>0.16115388454975099</v>
+        <v>0.24485156802299601</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11">
-        <v>5.3036896068016003E-2</v>
+      <c r="B11" s="1">
+        <v>0.17893471043357501</v>
       </c>
       <c r="C11" s="1">
-        <v>0.111322137619759</v>
+        <v>0.15585180874747101</v>
       </c>
       <c r="D11" s="1">
-        <v>8.8168669587429305E-2</v>
+        <v>0.105499427030701</v>
       </c>
       <c r="E11" s="1">
-        <v>0.102445857614599</v>
+        <v>8.7455500761162097E-2</v>
       </c>
       <c r="F11" s="1">
-        <v>2.4320422189222101E-2</v>
+        <v>9.6037941849076602E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12">
-        <v>7.7367915133582293E-2</v>
+      <c r="B12" s="1">
+        <v>9.0338684935777402E-2</v>
       </c>
       <c r="C12" s="1">
-        <v>0.31514126205477999</v>
+        <v>5.3628862915220302E-2</v>
       </c>
       <c r="D12" s="1">
-        <v>0.36980618721052599</v>
+        <v>6.8529774834357002E-2</v>
       </c>
       <c r="E12" s="1">
-        <v>0.34505404466883399</v>
+        <v>5.7967274718946797E-2</v>
       </c>
       <c r="F12" s="1">
-        <v>0.26924555962954999</v>
+        <v>9.0158905079726598E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
-      <c r="B13">
-        <v>6.4148239536454599E-2</v>
+      <c r="B13" s="1">
+        <v>9.27320711724791E-2</v>
       </c>
       <c r="C13" s="1">
-        <v>0.49255273211225598</v>
+        <v>2.7564757771104901E-2</v>
       </c>
       <c r="D13" s="1">
-        <v>0.47556033004235698</v>
+        <v>4.5836128698532201E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>0.56923891630180901</v>
+        <v>7.1338147512192293E-2</v>
       </c>
       <c r="F13" s="1">
-        <v>0.46726669627501899</v>
+        <v>5.9848557277288501E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14">
-        <v>0.33368181818292098</v>
+      <c r="B14" s="1">
+        <v>3.9317140542130501E-2</v>
       </c>
       <c r="C14" s="1">
-        <v>0.63417660574815005</v>
+        <v>2.68237890481655E-2</v>
       </c>
       <c r="D14" s="1">
-        <v>0.61169397701384998</v>
+        <v>3.1556962017103903E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>0.61917008120973205</v>
+        <v>6.8771334157419803E-2</v>
       </c>
       <c r="F14" s="1">
-        <v>0.61998166736207905</v>
+        <v>6.3926594414105101E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -8067,14 +9084,14 @@
       </c>
       <c r="B17">
         <f>AVERAGE(B2:F2)</f>
-        <v>0.12826232002703686</v>
+        <v>0.47660734054882703</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17">
         <f>AVERAGE(B9:F9)</f>
-        <v>0.32441322556399999</v>
+        <v>0.38968565539956995</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -8082,15 +9099,15 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <f>AVERAGE(B3:F3)</f>
-        <v>0.11521577061171033</v>
+        <f t="shared" ref="B18:B21" si="0">AVERAGE(B3:F3)</f>
+        <v>0.11011067595292796</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E18:E22" si="0">AVERAGE(B10:F10)</f>
-        <v>0.14288735612172593</v>
+        <f t="shared" ref="E18:E22" si="1">AVERAGE(B10:F10)</f>
+        <v>0.15337633108682519</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -8098,15 +9115,15 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <f>AVERAGE(B4:F4)</f>
-        <v>0.10111266851354897</v>
+        <f t="shared" si="0"/>
+        <v>0.13554706334072611</v>
       </c>
       <c r="D19" s="1">
         <v>3</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>7.585879661580508E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.12475587776439716</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -8114,15 +9131,15 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <f>AVERAGE(B5:F5)</f>
-        <v>0.14652123282950061</v>
+        <f t="shared" si="0"/>
+        <v>0.12262126794396215</v>
       </c>
       <c r="D20" s="1">
         <v>4</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
-        <v>0.27532299373945446</v>
+        <f t="shared" si="1"/>
+        <v>7.212470049680561E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -8130,15 +9147,15 @@
         <v>6</v>
       </c>
       <c r="B21">
-        <f>AVERAGE(B6:F6)</f>
-        <v>0.16997368084976899</v>
+        <f t="shared" si="0"/>
+        <v>0.12480658983983366</v>
       </c>
       <c r="D21" s="1">
         <v>5</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
-        <v>0.41375338285357915</v>
+        <f t="shared" si="1"/>
+        <v>5.9463932486319392E-2</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -8146,56 +9163,57 @@
         <v>6</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>0.5637408299033464</v>
+        <f t="shared" si="1"/>
+        <v>4.6079164035784957E-2</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I29" cm="1">
         <f t="array" ref="I29:M29">TRANSPOSE(B17:B21)</f>
-        <v>0.12826232002703686</v>
+        <v>0.47660734054882703</v>
       </c>
       <c r="J29">
-        <v>0.11521577061171033</v>
+        <v>0.11011067595292796</v>
       </c>
       <c r="K29">
-        <v>0.10111266851354897</v>
+        <v>0.13554706334072611</v>
       </c>
       <c r="L29">
-        <v>0.14652123282950061</v>
+        <v>0.12262126794396215</v>
       </c>
       <c r="M29">
-        <v>0.16997368084976899</v>
+        <v>0.12480658983983366</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I30" cm="1">
         <f t="array" ref="I30:N30">TRANSPOSE(E17:E22)</f>
-        <v>0.32441322556399999</v>
+        <v>0.38968565539956995</v>
       </c>
       <c r="J30">
-        <v>0.14288735612172593</v>
+        <v>0.15337633108682519</v>
       </c>
       <c r="K30">
-        <v>7.585879661580508E-2</v>
+        <v>0.12475587776439716</v>
       </c>
       <c r="L30">
-        <v>0.27532299373945446</v>
+        <v>7.212470049680561E-2</v>
       </c>
       <c r="M30">
-        <v>0.41375338285357915</v>
+        <v>5.9463932486319392E-2</v>
       </c>
       <c r="N30">
-        <v>0.5637408299033464</v>
+        <v>4.6079164035784957E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05EFA46A-66A1-4DD3-9CF2-7E67647E97FA}">
   <dimension ref="A1:AF86"/>
   <sheetViews>
@@ -10313,11 +11331,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F176BCA-B661-4AD4-9492-E5ACF33996F1}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="59" workbookViewId="0">
       <selection activeCell="M1" sqref="M1:P6"/>
     </sheetView>
   </sheetViews>
@@ -10944,7 +11962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C32A29-32CC-4B64-ABFF-95569F227936}">
   <dimension ref="A1:S44"/>
   <sheetViews>

</xml_diff>

<commit_message>
update for revised paper
</commit_message>
<xml_diff>
--- a/Paper data algorithm.xlsx
+++ b/Paper data algorithm.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/718232a78c2c86d3/Documenten/uni/uni documenten/MEP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2562" documentId="8_{E17B2787-9971-40C2-91F6-032D716F4A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C481B14A-FFF4-44C6-9A07-228C88423BA9}"/>
+  <xr:revisionPtr revIDLastSave="2261" documentId="8_{E17B2787-9971-40C2-91F6-032D716F4A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF8C14D0-5335-4E09-B613-63004E449F71}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{76006F6F-BB6B-4FCD-8E2D-5E202D6EDD84}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{76006F6F-BB6B-4FCD-8E2D-5E202D6EDD84}"/>
   </bookViews>
   <sheets>
     <sheet name="noise" sheetId="1" r:id="rId1"/>
     <sheet name="resolution" sheetId="2" r:id="rId2"/>
-    <sheet name="optimization revised" sheetId="7" r:id="rId3"/>
-    <sheet name="temps+inits" sheetId="3" r:id="rId4"/>
-    <sheet name="num metrics" sheetId="4" r:id="rId5"/>
-    <sheet name="optimization" sheetId="6" r:id="rId6"/>
-    <sheet name="right&amp;wrong" sheetId="5" r:id="rId7"/>
+    <sheet name="temps+inits" sheetId="3" r:id="rId3"/>
+    <sheet name="num metrics" sheetId="4" r:id="rId4"/>
+    <sheet name="optimization" sheetId="6" r:id="rId5"/>
+    <sheet name="right&amp;wrong" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="112">
   <si>
     <t>stat/var noise</t>
   </si>
@@ -425,154 +424,15 @@
   <si>
     <t>Score for true system</t>
   </si>
-  <si>
-    <t>Double iterations</t>
-  </si>
-  <si>
-    <t>triple iterations</t>
-  </si>
-  <si>
-    <t>Double iter</t>
-  </si>
-  <si>
-    <t>Triple iter</t>
-  </si>
-  <si>
-    <t>#SMAPE 0.1 results</t>
-  </si>
-  <si>
-    <t>#SMAPE 0.2 results</t>
-  </si>
-  <si>
-    <t>#SMAPE 0.4 results</t>
-  </si>
-  <si>
-    <t>Chemfit parameters for a SMAPE of 0.05</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>16716</t>
-  </si>
-  <si>
-    <t>14893</t>
-  </si>
-  <si>
-    <t>18431</t>
-  </si>
-  <si>
-    <t>15589</t>
-  </si>
-  <si>
-    <t>12232</t>
-  </si>
-  <si>
-    <t>24725</t>
-  </si>
-  <si>
-    <t>21096</t>
-  </si>
-  <si>
-    <t>11225</t>
-  </si>
-  <si>
-    <t>12755</t>
-  </si>
-  <si>
-    <t>13550</t>
-  </si>
-  <si>
-    <t>24555</t>
-  </si>
-  <si>
-    <t>14247</t>
-  </si>
-  <si>
-    <t>19395</t>
-  </si>
-  <si>
-    <t>22674</t>
-  </si>
-  <si>
-    <t>28023</t>
-  </si>
-  <si>
-    <t>12455</t>
-  </si>
-  <si>
-    <t>35554</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>yield</t>
-  </si>
-  <si>
-    <t>cat conc</t>
-  </si>
-  <si>
-    <t>pressure</t>
-  </si>
-  <si>
-    <t>substrate conc</t>
-  </si>
-  <si>
-    <t>temperature</t>
-  </si>
-  <si>
-    <t>True parameters</t>
-  </si>
-  <si>
-    <t>SMAPE 0,05</t>
-  </si>
-  <si>
-    <t>SMAPE 0,10</t>
-  </si>
-  <si>
-    <t>SMAPE 0,20</t>
-  </si>
-  <si>
-    <t>SMAPE 0,4</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00000000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -889,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -984,11 +844,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1018,7 +876,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1080,7 +938,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1130,10 +988,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>resolution!$K$2:$K$12</c:f>
+              <c:f>resolution!$K$2:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>120</c:v>
                 </c:pt>
@@ -1166,16 +1024,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>resolution!$L$2:$L$12</c:f>
+              <c:f>resolution!$L$2:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>9.9069306164461402E-3</c:v>
                 </c:pt>
@@ -1208,6 +1069,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>7.4038794524886195E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.30262494241506599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1259,10 +1123,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>resolution!$K$2:$K$12</c:f>
+              <c:f>resolution!$K$2:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>120</c:v>
                 </c:pt>
@@ -1295,16 +1159,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>resolution!$M$2:$M$12</c:f>
+              <c:f>resolution!$M$2:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.15184317161043559</c:v>
                 </c:pt>
@@ -1337,6 +1204,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.2901396885429634</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.28560059863407572</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1345,219 +1215,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8BCE-4FCF-9F3E-37A65F1984D9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>resolution!$N$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Double iter</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>resolution!$K$2:$K$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>resolution!$N$2:$N$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>5.5892299346689135E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.5602152249516387E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.6273886462089043E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.10146021097734037</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.13722927374678071</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AB29-4665-A1B1-BF16A0937D54}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>resolution!$O$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Triple iter</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>resolution!$K$2:$K$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>resolution!$O$2:$O$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>3.4840100173685939E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.2173074449784987E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-AB29-4665-A1B1-BF16A0937D54}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1645,7 +1302,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1683,7 +1340,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718606680"/>
@@ -1762,7 +1419,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1800,7 +1457,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718606352"/>
@@ -1842,7 +1499,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1879,7 +1536,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1893,7 +1550,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1960,7 +1617,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2004,19 +1661,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>0.47660734054882703</c:v>
+                  <c:v>0.12826232002703686</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11011067595292796</c:v>
+                  <c:v>0.11521577061171033</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13554706334072611</c:v>
+                  <c:v>0.10111266851354897</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.12262126794396215</c:v>
+                  <c:v>0.14652123282950061</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.12480658983983366</c:v>
+                  <c:v>0.16997368084976899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2190,7 +1847,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2227,7 +1884,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718065736"/>
@@ -2307,7 +1964,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2345,7 +2002,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718068360"/>
@@ -2393,7 +2050,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2407,7 +2064,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2502,7 +2159,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2546,22 +2203,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="1">
-                  <c:v>0.38968565539956995</c:v>
+                  <c:v>0.32441322556399999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15337633108682519</c:v>
+                  <c:v>0.14288735612172593</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12475587776439716</c:v>
+                  <c:v>7.585879661580508E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.212470049680561E-2</c:v>
+                  <c:v>0.27532299373945446</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.9463932486319392E-2</c:v>
+                  <c:v>0.41375338285357915</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6079164035784957E-2</c:v>
+                  <c:v>0.5637408299033464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2733,7 +2390,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2770,7 +2427,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="653071328"/>
@@ -2849,7 +2506,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2887,7 +2544,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="653071000"/>
@@ -2935,7 +2592,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2949,7 +2606,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2986,7 +2643,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3671,7 +3328,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="688023240"/>
@@ -3730,7 +3387,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="688026520"/>
@@ -3772,7 +3429,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3809,7 +3466,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6256,12 +5913,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7410,19 +7063,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B1E574-918A-43D0-93C9-C767A11D8FF9}">
-  <dimension ref="A1:AB37"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R5" sqref="Q5:R5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="12" max="12" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -7435,14 +7087,8 @@
       <c r="M1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
-        <v>114</v>
-      </c>
-      <c r="O1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>120</v>
       </c>
@@ -7472,53 +7118,45 @@
         <f>AVERAGE(B15:F15)</f>
         <v>0.15184317161043559</v>
       </c>
-      <c r="N2">
-        <f>AVERAGE(B29:F29)</f>
-        <v>5.5892299346689135E-2</v>
-      </c>
-      <c r="O2">
-        <f>AVERAGE(B36:F36)</f>
-        <v>3.4840100173685939E-2</v>
-      </c>
-      <c r="Q2" cm="1">
-        <f t="array" ref="Q2:AB5">TRANSPOSE(L2:O13)</f>
+      <c r="O2" cm="1">
+        <f t="array" ref="O2:Z3">TRANSPOSE(L2:M13)</f>
         <v>9.9069306164461402E-3</v>
       </c>
+      <c r="P2">
+        <v>1.9077525198916999E-2</v>
+      </c>
+      <c r="Q2">
+        <v>2.1075758971819299E-2</v>
+      </c>
       <c r="R2">
-        <v>1.9077525198916999E-2</v>
+        <v>3.5933315828482124E-2</v>
       </c>
       <c r="S2">
-        <v>2.1075758971819299E-2</v>
+        <v>2.5965459400004564E-2</v>
       </c>
       <c r="T2">
-        <v>3.5933315828482124E-2</v>
+        <v>3.7405057350412038E-2</v>
       </c>
       <c r="U2">
-        <v>2.5965459400004564E-2</v>
+        <v>5.3036896068016003E-2</v>
       </c>
       <c r="V2">
-        <v>3.7405057350412038E-2</v>
+        <v>4.5773000409559797E-2</v>
       </c>
       <c r="W2">
-        <v>5.3036896068016003E-2</v>
+        <v>5.2234662828366897E-2</v>
       </c>
       <c r="X2">
-        <v>4.5773000409559797E-2</v>
+        <v>0.120728141436048</v>
       </c>
       <c r="Y2">
-        <v>5.2234662828366897E-2</v>
+        <v>7.4038794524886195E-2</v>
       </c>
       <c r="Z2">
-        <v>0.120728141436048</v>
-      </c>
-      <c r="AA2">
-        <v>7.4038794524886195E-2</v>
-      </c>
-      <c r="AB2">
         <v>0.30262494241506599</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>60</v>
       </c>
@@ -7548,52 +7186,44 @@
         <f t="shared" ref="M3:M13" si="1">AVERAGE(B16:F16)</f>
         <v>0.102350495769891</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N4" si="2">AVERAGE(B30:F30)</f>
-        <v>4.5602152249516387E-2</v>
-      </c>
       <c r="O3">
-        <f>AVERAGE(B37:F37)</f>
-        <v>5.2173074449784987E-2</v>
+        <v>0.15184317161043559</v>
+      </c>
+      <c r="P3">
+        <v>0.102350495769891</v>
       </c>
       <c r="Q3">
-        <v>0.15184317161043559</v>
+        <v>9.0212364833213848E-2</v>
       </c>
       <c r="R3">
-        <v>0.102350495769891</v>
+        <v>0.10222289006575935</v>
       </c>
       <c r="S3">
-        <v>9.0212364833213848E-2</v>
+        <v>0.13154454769095564</v>
       </c>
       <c r="T3">
-        <v>0.10222289006575935</v>
+        <v>0.1380056493489962</v>
       </c>
       <c r="U3">
-        <v>0.13154454769095564</v>
+        <v>0.12829677436831735</v>
       </c>
       <c r="V3">
-        <v>0.1380056493489962</v>
+        <v>0.13536845499994438</v>
       </c>
       <c r="W3">
-        <v>0.12829677436831735</v>
+        <v>0.2826345705229984</v>
       </c>
       <c r="X3">
-        <v>0.13536845499994438</v>
+        <v>0.23483273174420888</v>
       </c>
       <c r="Y3">
-        <v>0.2826345705229984</v>
+        <v>0.2901396885429634</v>
       </c>
       <c r="Z3">
-        <v>0.23483273174420888</v>
-      </c>
-      <c r="AA3">
-        <v>0.2901396885429634</v>
-      </c>
-      <c r="AB3">
         <v>0.28560059863407572</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
@@ -7623,48 +7253,8 @@
         <f t="shared" si="1"/>
         <v>9.0212364833213848E-2</v>
       </c>
-      <c r="N4">
-        <f t="shared" si="2"/>
-        <v>5.6273886462089043E-2</v>
-      </c>
-      <c r="Q4">
-        <v>5.5892299346689135E-2</v>
-      </c>
-      <c r="R4">
-        <v>4.5602152249516387E-2</v>
-      </c>
-      <c r="S4">
-        <v>5.6273886462089043E-2</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0.10146021097734037</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0.13722927374678071</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>25</v>
       </c>
@@ -7694,44 +7284,8 @@
         <f t="shared" si="1"/>
         <v>0.10222289006575935</v>
       </c>
-      <c r="Q5">
-        <v>3.4840100173685939E-2</v>
-      </c>
-      <c r="R5">
-        <v>5.2173074449784987E-2</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20</v>
       </c>
@@ -7762,7 +7316,7 @@
         <v>0.13154454769095564</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>15</v>
       </c>
@@ -7792,12 +7346,8 @@
         <f t="shared" si="1"/>
         <v>0.1380056493489962</v>
       </c>
-      <c r="N7">
-        <f>AVERAGE(B32:F32)</f>
-        <v>0.10146021097734037</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
@@ -7828,7 +7378,7 @@
         <v>0.12829677436831735</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7858,12 +7408,8 @@
         <f t="shared" si="1"/>
         <v>0.13536845499994438</v>
       </c>
-      <c r="N9">
-        <f>AVERAGE(B33:F33)</f>
-        <v>0.13722927374678071</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -7894,7 +7440,7 @@
         <v>0.2826345705229984</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -7925,7 +7471,7 @@
         <v>0.23483273174420888</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
@@ -7956,7 +7502,7 @@
         <v>0.2901396885429634</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -7987,12 +7533,12 @@
         <v>0.28560059863407572</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>120</v>
       </c>
@@ -8012,7 +7558,7 @@
         <v>0.18089594150018901</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>60</v>
       </c>
@@ -8232,155 +7778,12 @@
         <v>8.8135208074904603E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>112</v>
-      </c>
-    </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>120</v>
-      </c>
-      <c r="B29" s="1">
-        <v>6.0776284874391198E-2</v>
-      </c>
-      <c r="C29" s="1">
-        <v>4.0230590071408799E-2</v>
-      </c>
-      <c r="D29" s="1">
-        <v>8.0670378581654795E-2</v>
-      </c>
-      <c r="E29" s="1">
-        <v>6.9328505660221806E-2</v>
-      </c>
-      <c r="F29" s="1">
-        <v>2.8455737545769098E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>60</v>
-      </c>
-      <c r="B30" s="1">
-        <v>4.5692758027233001E-2</v>
-      </c>
-      <c r="C30" s="1">
-        <v>3.6356991775736799E-2</v>
-      </c>
-      <c r="D30" s="1">
-        <v>6.2280883904184903E-2</v>
-      </c>
-      <c r="E30" s="1">
-        <v>3.1061277676646501E-2</v>
-      </c>
-      <c r="F30" s="1">
-        <v>5.2618849863780702E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1">
-        <v>5.4644962601521803E-2</v>
-      </c>
-      <c r="C31" s="1">
-        <v>7.8354039849733298E-2</v>
-      </c>
-      <c r="D31" s="1">
-        <v>3.3063891388189499E-2</v>
-      </c>
-      <c r="E31" s="1">
-        <v>4.4105702800082199E-2</v>
-      </c>
-      <c r="F31" s="1">
-        <v>7.1200835670918394E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>15</v>
-      </c>
-      <c r="B32" s="1">
-        <v>5.7104750677369899E-2</v>
-      </c>
-      <c r="C32" s="1">
-        <v>6.7770013850707703E-2</v>
-      </c>
-      <c r="D32" s="1">
-        <v>4.0686977880168299E-2</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0.184739173615421</v>
-      </c>
-      <c r="F32" s="1">
-        <v>0.15700013886303499</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>8</v>
-      </c>
-      <c r="B33" s="1">
-        <v>0.13883319097482799</v>
-      </c>
-      <c r="C33" s="1">
-        <v>0.15868218691062699</v>
-      </c>
-      <c r="D33" s="1">
-        <v>9.9446665779917606E-2</v>
-      </c>
-      <c r="E33" s="1">
-        <v>0.118764957611982</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0.17041936745654901</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>120</v>
-      </c>
-      <c r="B36" s="1">
-        <v>2.4728097479248499E-2</v>
-      </c>
-      <c r="C36" s="1">
-        <v>2.93592467550042E-2</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1.8120420990648201E-2</v>
-      </c>
-      <c r="E36" s="1">
-        <v>6.1660616586454199E-2</v>
-      </c>
-      <c r="F36" s="1">
-        <v>4.0332119057074602E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>60</v>
-      </c>
-      <c r="B37" s="1">
-        <v>2.9922403858221799E-2</v>
-      </c>
-      <c r="C37" s="1">
-        <v>5.42980200042096E-2</v>
-      </c>
-      <c r="D37" s="1">
-        <v>5.5705359528884002E-2</v>
-      </c>
-      <c r="E37" s="1">
-        <v>3.09711762972831E-2</v>
-      </c>
-      <c r="F37" s="1">
-        <v>8.9968412560326394E-2</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8390,431 +7793,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB486C5-C788-456E-AE38-E770553E351F}">
-  <dimension ref="A1:K55"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="39">
-        <v>3.335</v>
-      </c>
-      <c r="G2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H2" t="s">
-        <v>149</v>
-      </c>
-      <c r="I2" t="s">
-        <v>150</v>
-      </c>
-      <c r="J2" t="s">
-        <v>151</v>
-      </c>
-      <c r="K2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="39">
-        <v>1.98</v>
-      </c>
-      <c r="F3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G3">
-        <v>0.78800000000000003</v>
-      </c>
-      <c r="H3">
-        <v>0.48080000000000001</v>
-      </c>
-      <c r="I3">
-        <v>50</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>396.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="39">
-        <v>1.2589999999999999</v>
-      </c>
-      <c r="F4" t="s">
-        <v>154</v>
-      </c>
-      <c r="G4">
-        <v>0.79090000000000005</v>
-      </c>
-      <c r="H4">
-        <v>0.50649999999999995</v>
-      </c>
-      <c r="I4">
-        <v>50</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>406.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B5" s="39">
-        <v>4.0990000000000002</v>
-      </c>
-      <c r="F5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G5">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="H5">
-        <v>0.57969999999999999</v>
-      </c>
-      <c r="I5">
-        <v>50</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>387.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="39">
-        <v>1.921</v>
-      </c>
-      <c r="F6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G6">
-        <v>0.93759999999999999</v>
-      </c>
-      <c r="H6">
-        <v>0.1</v>
-      </c>
-      <c r="I6">
-        <v>50</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B7" s="38">
-        <v>32.880000000000003</v>
-      </c>
-      <c r="F7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G7">
-        <v>0.81679999999999997</v>
-      </c>
-      <c r="H7">
-        <v>0.16350000000000001</v>
-      </c>
-      <c r="I7">
-        <v>50</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>327.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8">
-        <v>17041</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9">
-        <v>14699</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10">
-        <v>17180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B11">
-        <v>11794</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B12">
-        <v>12290</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13">
-        <v>23902</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>3.036</v>
-      </c>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>2.1520000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>1.946</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18.32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>1.8879999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>48.01</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>13.92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>0.56899999999999995</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>0.26600000000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>0.47699999999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>2.8959999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>40.78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>5806</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>1.3740000000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>8.0719999999999992</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>5.7439999999999998</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>1.966</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>1645</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>146</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BECF976-1F9D-4521-BFCB-8389D9F3AE5F}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30:N30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8832,19 +7815,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>0.45001318515774102</v>
+        <v>0.15794782190330101</v>
       </c>
       <c r="C2" s="1">
-        <v>0.451111005796686</v>
+        <v>0.135929624025662</v>
       </c>
       <c r="D2" s="1">
-        <v>0.51519663046880404</v>
+        <v>0.124953451942575</v>
       </c>
       <c r="E2" s="1">
-        <v>0.54589874080093403</v>
+        <v>0.12896263949139999</v>
       </c>
       <c r="F2" s="1">
-        <v>0.42081714051996999</v>
+        <v>9.3518062772246294E-2</v>
       </c>
       <c r="I2">
         <v>363.39299999999997</v>
@@ -8854,20 +7837,20 @@
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>4.2905398699690699E-2</v>
+      <c r="B3">
+        <v>0.15135796075552699</v>
       </c>
       <c r="C3" s="1">
-        <v>0.119204489253286</v>
+        <v>0.105007070406527</v>
       </c>
       <c r="D3" s="1">
-        <v>0.161434982649105</v>
+        <v>9.5401381060959897E-2</v>
       </c>
       <c r="E3" s="1">
-        <v>9.6502101484839106E-2</v>
+        <v>5.7004650254663801E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>0.13050640767771901</v>
+        <v>0.167307790580874</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
@@ -8877,20 +7860,20 @@
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
-        <v>6.0849093685008099E-2</v>
+      <c r="B4">
+        <v>0.10354473058275999</v>
       </c>
       <c r="C4" s="1">
-        <v>0.156610526030558</v>
+        <v>0.13345832691191101</v>
       </c>
       <c r="D4" s="1">
-        <v>0.174373660446316</v>
+        <v>5.7627767914828397E-2</v>
       </c>
       <c r="E4" s="1">
-        <v>9.3212351034178395E-2</v>
+        <v>5.44234707844145E-2</v>
       </c>
       <c r="F4" s="1">
-        <v>0.19268968550757001</v>
+        <v>0.15650904637383101</v>
       </c>
       <c r="I4" t="s">
         <v>20</v>
@@ -8900,20 +7883,20 @@
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
-        <v>0.17639374508299499</v>
+      <c r="B5">
+        <v>0.19029847657617399</v>
       </c>
       <c r="C5" s="1">
-        <v>8.9200853387824505E-2</v>
+        <v>0.132628257675839</v>
       </c>
       <c r="D5" s="1">
-        <v>0.14301509580456301</v>
+        <v>0.143963903523943</v>
       </c>
       <c r="E5" s="1">
-        <v>0.11020204974744099</v>
+        <v>0.14145528030861501</v>
       </c>
       <c r="F5" s="1">
-        <v>9.4294595696987296E-2</v>
+        <v>0.124260246062932</v>
       </c>
       <c r="I5" t="s">
         <v>21</v>
@@ -8923,20 +7906,20 @@
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.102792690730237</v>
+      <c r="B6">
+        <v>0.176954265049521</v>
       </c>
       <c r="C6" s="1">
-        <v>0.104030767381089</v>
+        <v>0.275619628560764</v>
       </c>
       <c r="D6" s="1">
-        <v>0.18112636036377999</v>
+        <v>0.123852896654535</v>
       </c>
       <c r="E6" s="1">
-        <v>0.16226486287007699</v>
+        <v>0.16236967387731499</v>
       </c>
       <c r="F6" s="1">
-        <v>7.3818267853985306E-2</v>
+        <v>0.11107194010671</v>
       </c>
       <c r="I6" t="s">
         <v>22</v>
@@ -8951,20 +7934,20 @@
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="1">
-        <v>0.305099204962472</v>
+      <c r="B9">
+        <v>0.28130613318018299</v>
       </c>
       <c r="C9" s="1">
-        <v>0.44407054607834401</v>
+        <v>0.27609094167620701</v>
       </c>
       <c r="D9" s="1">
-        <v>0.40911367953584599</v>
+        <v>0.34363120854850399</v>
       </c>
       <c r="E9" s="1">
-        <v>0.377778342613378</v>
+        <v>0.32686950657540498</v>
       </c>
       <c r="F9" s="1">
-        <v>0.41236650380780998</v>
+        <v>0.39416833783970101</v>
       </c>
       <c r="I9" t="s">
         <v>31</v>
@@ -8974,100 +7957,100 @@
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="1">
-        <v>0.113788948412263</v>
+      <c r="B10">
+        <v>0.14761230951581999</v>
       </c>
       <c r="C10" s="1">
-        <v>8.3113454945618906E-2</v>
+        <v>0.223577999164978</v>
       </c>
       <c r="D10" s="1">
-        <v>0.12551949139320501</v>
+        <v>0.11786896607290701</v>
       </c>
       <c r="E10" s="1">
-        <v>0.19960819266004301</v>
+        <v>6.4223621305173603E-2</v>
       </c>
       <c r="F10" s="1">
-        <v>0.24485156802299601</v>
+        <v>0.16115388454975099</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="1">
-        <v>0.17893471043357501</v>
+      <c r="B11">
+        <v>5.3036896068016003E-2</v>
       </c>
       <c r="C11" s="1">
-        <v>0.15585180874747101</v>
+        <v>0.111322137619759</v>
       </c>
       <c r="D11" s="1">
-        <v>0.105499427030701</v>
+        <v>8.8168669587429305E-2</v>
       </c>
       <c r="E11" s="1">
-        <v>8.7455500761162097E-2</v>
+        <v>0.102445857614599</v>
       </c>
       <c r="F11" s="1">
-        <v>9.6037941849076602E-2</v>
+        <v>2.4320422189222101E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" s="1">
-        <v>9.0338684935777402E-2</v>
+      <c r="B12">
+        <v>7.7367915133582293E-2</v>
       </c>
       <c r="C12" s="1">
-        <v>5.3628862915220302E-2</v>
+        <v>0.31514126205477999</v>
       </c>
       <c r="D12" s="1">
-        <v>6.8529774834357002E-2</v>
+        <v>0.36980618721052599</v>
       </c>
       <c r="E12" s="1">
-        <v>5.7967274718946797E-2</v>
+        <v>0.34505404466883399</v>
       </c>
       <c r="F12" s="1">
-        <v>9.0158905079726598E-2</v>
+        <v>0.26924555962954999</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
-      <c r="B13" s="1">
-        <v>9.27320711724791E-2</v>
+      <c r="B13">
+        <v>6.4148239536454599E-2</v>
       </c>
       <c r="C13" s="1">
-        <v>2.7564757771104901E-2</v>
+        <v>0.49255273211225598</v>
       </c>
       <c r="D13" s="1">
-        <v>4.5836128698532201E-2</v>
+        <v>0.47556033004235698</v>
       </c>
       <c r="E13" s="1">
-        <v>7.1338147512192293E-2</v>
+        <v>0.56923891630180901</v>
       </c>
       <c r="F13" s="1">
-        <v>5.9848557277288501E-2</v>
+        <v>0.46726669627501899</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="1">
-        <v>3.9317140542130501E-2</v>
+      <c r="B14">
+        <v>0.33368181818292098</v>
       </c>
       <c r="C14" s="1">
-        <v>2.68237890481655E-2</v>
+        <v>0.63417660574815005</v>
       </c>
       <c r="D14" s="1">
-        <v>3.1556962017103903E-2</v>
+        <v>0.61169397701384998</v>
       </c>
       <c r="E14" s="1">
-        <v>6.8771334157419803E-2</v>
+        <v>0.61917008120973205</v>
       </c>
       <c r="F14" s="1">
-        <v>6.3926594414105101E-2</v>
+        <v>0.61998166736207905</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -9084,14 +8067,14 @@
       </c>
       <c r="B17">
         <f>AVERAGE(B2:F2)</f>
-        <v>0.47660734054882703</v>
+        <v>0.12826232002703686</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17">
         <f>AVERAGE(B9:F9)</f>
-        <v>0.38968565539956995</v>
+        <v>0.32441322556399999</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -9099,15 +8082,15 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <f t="shared" ref="B18:B21" si="0">AVERAGE(B3:F3)</f>
-        <v>0.11011067595292796</v>
+        <f>AVERAGE(B3:F3)</f>
+        <v>0.11521577061171033</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E18:E22" si="1">AVERAGE(B10:F10)</f>
-        <v>0.15337633108682519</v>
+        <f t="shared" ref="E18:E22" si="0">AVERAGE(B10:F10)</f>
+        <v>0.14288735612172593</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -9115,15 +8098,15 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
-        <v>0.13554706334072611</v>
+        <f>AVERAGE(B4:F4)</f>
+        <v>0.10111266851354897</v>
       </c>
       <c r="D19" s="1">
         <v>3</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
-        <v>0.12475587776439716</v>
+        <f t="shared" si="0"/>
+        <v>7.585879661580508E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -9131,15 +8114,15 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
-        <v>0.12262126794396215</v>
+        <f>AVERAGE(B5:F5)</f>
+        <v>0.14652123282950061</v>
       </c>
       <c r="D20" s="1">
         <v>4</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
-        <v>7.212470049680561E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.27532299373945446</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -9147,15 +8130,15 @@
         <v>6</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
-        <v>0.12480658983983366</v>
+        <f>AVERAGE(B6:F6)</f>
+        <v>0.16997368084976899</v>
       </c>
       <c r="D21" s="1">
         <v>5</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
-        <v>5.9463932486319392E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.41375338285357915</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -9163,57 +8146,56 @@
         <v>6</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
-        <v>4.6079164035784957E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.5637408299033464</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I29" cm="1">
         <f t="array" ref="I29:M29">TRANSPOSE(B17:B21)</f>
-        <v>0.47660734054882703</v>
+        <v>0.12826232002703686</v>
       </c>
       <c r="J29">
-        <v>0.11011067595292796</v>
+        <v>0.11521577061171033</v>
       </c>
       <c r="K29">
-        <v>0.13554706334072611</v>
+        <v>0.10111266851354897</v>
       </c>
       <c r="L29">
-        <v>0.12262126794396215</v>
+        <v>0.14652123282950061</v>
       </c>
       <c r="M29">
-        <v>0.12480658983983366</v>
+        <v>0.16997368084976899</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I30" cm="1">
         <f t="array" ref="I30:N30">TRANSPOSE(E17:E22)</f>
-        <v>0.38968565539956995</v>
+        <v>0.32441322556399999</v>
       </c>
       <c r="J30">
-        <v>0.15337633108682519</v>
+        <v>0.14288735612172593</v>
       </c>
       <c r="K30">
-        <v>0.12475587776439716</v>
+        <v>7.585879661580508E-2</v>
       </c>
       <c r="L30">
-        <v>7.212470049680561E-2</v>
+        <v>0.27532299373945446</v>
       </c>
       <c r="M30">
-        <v>5.9463932486319392E-2</v>
+        <v>0.41375338285357915</v>
       </c>
       <c r="N30">
-        <v>4.6079164035784957E-2</v>
+        <v>0.5637408299033464</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05EFA46A-66A1-4DD3-9CF2-7E67647E97FA}">
   <dimension ref="A1:AF86"/>
   <sheetViews>
@@ -11331,11 +10313,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F176BCA-B661-4AD4-9492-E5ACF33996F1}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView zoomScale="59" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1:P6"/>
     </sheetView>
   </sheetViews>
@@ -11962,7 +10944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C32A29-32CC-4B64-ABFF-95569F227936}">
   <dimension ref="A1:S44"/>
   <sheetViews>

</xml_diff>